<commit_message>
update figure in response to reviewer comments
</commit_message>
<xml_diff>
--- a/great_expectations_data/data/consistency_data.xlsx
+++ b/great_expectations_data/data/consistency_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielsond/code/midla/great_expectations/great_expectations_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2372B37D-010A-804E-BB12-0556ADDBF373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C139F16A-85BD-324D-96CB-E16F2C58E49C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1640" windowWidth="19880" windowHeight="19080" xr2:uid="{6F7F254C-19AA-0941-A36B-092038D3ED16}"/>
+    <workbookView xWindow="33960" yWindow="10120" windowWidth="20640" windowHeight="25940" xr2:uid="{6F7F254C-19AA-0941-A36B-092038D3ED16}"/>
   </bookViews>
   <sheets>
     <sheet name="keren_fmri_data" sheetId="1" r:id="rId1"/>
     <sheet name="ng_data" sheetId="2" r:id="rId2"/>
+    <sheet name="zhang_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="173">
   <si>
     <t>label</t>
   </si>
@@ -108,9 +109,6 @@
     <t>Affective</t>
   </si>
   <si>
-    <t>AID</t>
-  </si>
-  <si>
     <t>Chandrasekhar Pammi et al. (2015)</t>
   </si>
   <si>
@@ -523,13 +521,46 @@
   </si>
   <si>
     <t>Indicating the sex of faces that were fearful, angry, sad, happy, neutral, or scrambled</t>
+  </si>
+  <si>
+    <t>Canli et al. (2004)</t>
+  </si>
+  <si>
+    <t>Derntl et al. (2011)</t>
+  </si>
+  <si>
+    <t>Epstein et al. (2006)</t>
+  </si>
+  <si>
+    <t>Kumar et al. (2008)</t>
+  </si>
+  <si>
+    <t>McCabe et al. (2009)</t>
+  </si>
+  <si>
+    <t>Mitterschiffthaler et al. (2003)</t>
+  </si>
+  <si>
+    <t>Emotional word processing</t>
+  </si>
+  <si>
+    <t>positive &gt; baseline</t>
+  </si>
+  <si>
+    <t>temporance difference</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Affective Incentive Delay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -540,21 +571,30 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -589,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -599,6 +639,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +957,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1027,7 +1068,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>172</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>15</v>
@@ -1038,65 +1079,65 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>15</v>
@@ -1107,13 +1148,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -1130,13 +1171,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -1153,19 +1194,19 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>12</v>
@@ -1176,7 +1217,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1188,18 +1229,18 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1222,7 +1263,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -1245,7 +1286,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1268,7 +1309,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1291,19 +1332,19 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
@@ -1314,13 +1355,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
@@ -1337,13 +1378,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>10</v>
@@ -1360,13 +1401,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
@@ -1375,67 +1416,67 @@
         <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
@@ -1452,19 +1493,19 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>12</v>
@@ -1475,30 +1516,30 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
@@ -1521,7 +1562,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -1544,7 +1585,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -1562,18 +1603,18 @@
         <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>10</v>
@@ -1590,13 +1631,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>10</v>
@@ -1608,18 +1649,18 @@
         <v>12</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>10</v>
@@ -1636,13 +1677,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>10</v>
@@ -1654,18 +1695,18 @@
         <v>15</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>10</v>
@@ -1682,7 +1723,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>8</v>
@@ -1705,7 +1746,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>8</v>
@@ -1728,7 +1769,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>8</v>
@@ -1751,7 +1792,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>8</v>
@@ -1774,7 +1815,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>8</v>
@@ -1789,15 +1830,15 @@
         <v>11</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>8</v>
@@ -1820,7 +1861,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>8</v>
@@ -1832,7 +1873,7 @@
         <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>12</v>
@@ -1843,42 +1884,42 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>12</v>
@@ -1889,30 +1930,30 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="F43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>8</v>
@@ -1930,18 +1971,18 @@
         <v>12</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>10</v>
@@ -1950,15 +1991,15 @@
         <v>11</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>8</v>
@@ -1970,7 +2011,7 @@
         <v>10</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>12</v>
@@ -1981,13 +2022,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>10</v>
@@ -2004,7 +2045,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>8</v>
@@ -2016,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>15</v>
@@ -2027,7 +2068,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>8</v>
@@ -2039,7 +2080,7 @@
         <v>10</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>12</v>
@@ -2050,7 +2091,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>8</v>
@@ -2062,27 +2103,27 @@
         <v>10</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>11</v>
@@ -2096,16 +2137,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>11</v>
@@ -2119,7 +2160,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>8</v>
@@ -2128,21 +2169,21 @@
         <v>9</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>8</v>
@@ -2165,7 +2206,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>8</v>
@@ -2183,18 +2224,18 @@
         <v>15</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>10</v>
@@ -2211,7 +2252,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>8</v>
@@ -2223,18 +2264,18 @@
         <v>10</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>8</v>
@@ -2246,30 +2287,30 @@
         <v>10</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>15</v>
@@ -2280,25 +2321,25 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2311,7 +2352,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I45"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2339,56 +2380,56 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -2397,15 +2438,15 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -2426,15 +2467,15 @@
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -2452,18 +2493,18 @@
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -2481,192 +2522,192 @@
         <v>12</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" t="s">
         <v>111</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -2678,53 +2719,53 @@
         <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -2736,24 +2777,24 @@
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -2765,227 +2806,227 @@
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" t="s">
         <v>132</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -2997,111 +3038,111 @@
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -3113,53 +3154,53 @@
         <v>23</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -3171,53 +3212,53 @@
         <v>23</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>8</v>
@@ -3229,53 +3270,53 @@
         <v>23</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>8</v>
@@ -3287,24 +3328,24 @@
         <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>8</v>
@@ -3316,181 +3357,181 @@
         <v>23</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="F40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>12</v>
@@ -3499,15 +3540,15 @@
         <v>16</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>8</v>
@@ -3519,7 +3560,7 @@
         <v>23</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>12</v>
@@ -3528,15 +3569,15 @@
         <v>16</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>8</v>
@@ -3548,77 +3589,281 @@
         <v>23</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="1" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC40004F-BBF4-C14F-97E9-23A17E21E909}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>162</v>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>